<commit_message>
excel parsing theoretically done
</commit_message>
<xml_diff>
--- a/core/assets/levels/LevelTemplate.xlsx
+++ b/core/assets/levels/LevelTemplate.xlsx
@@ -47,9 +47,6 @@
     <t>Song Genre</t>
   </si>
   <si>
-    <t>Each lane cell represents 50 in-game miles</t>
-  </si>
-  <si>
     <t>Specifications</t>
   </si>
   <si>
@@ -257,9 +254,6 @@
     <t>To end each block, still put "END" in the last row in the corresponding events column.</t>
   </si>
   <si>
-    <t>Padding between enemies defines how close together two rows will appear in-game.</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <u/>
@@ -366,13 +360,19 @@
   </si>
   <si>
     <t>Grill End</t>
+  </si>
+  <si>
+    <t>Less padding: 1 cell = 3 miles / Normal padding: 1 cell = 5 miles / More padding: 1 cell = 8 miles</t>
+  </si>
+  <si>
+    <t>An average level is roughly 200 miles (40 rows total with normal padding).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -423,6 +423,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -450,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -461,15 +475,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -750,7 +766,7 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -771,39 +787,39 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="3">
         <v>3</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -811,16 +827,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>4</v>
@@ -840,9 +856,9 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="12">
+        <v>27</v>
+      </c>
+      <c r="D5" s="11">
         <v>0</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -853,29 +869,29 @@
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="8"/>
+      <c r="A7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="13"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="6"/>
       <c r="H8" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="6"/>
     </row>
@@ -888,7 +904,7 @@
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D12" s="6"/>
       <c r="H12" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -902,7 +918,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
@@ -937,7 +953,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
@@ -950,7 +966,7 @@
       <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B21" s="4"/>
@@ -962,15 +978,15 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
-        <v>27</v>
+      <c r="A23" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
@@ -978,7 +994,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="5"/>
@@ -986,7 +1002,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
@@ -994,18 +1010,18 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
-        <v>40</v>
+      <c r="A27" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
@@ -1013,22 +1029,21 @@
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
-        <v>48</v>
+      <c r="A28" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="9"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
     </row>
     <row r="30" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="10" t="s">
-        <v>7</v>
+      <c r="A30" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="5"/>
@@ -1036,7 +1051,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="5"/>
@@ -1044,23 +1059,23 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
-        <v>23</v>
+      <c r="A33" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
-        <v>42</v>
+      <c r="A34" s="14" t="s">
+        <v>55</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="5"/>
@@ -1068,7 +1083,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="5"/>
@@ -1076,7 +1091,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="5"/>
@@ -1084,7 +1099,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="5"/>
@@ -1092,21 +1107,21 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="10"/>
+      <c r="A39" s="9"/>
       <c r="B39" s="4"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="10" t="s">
-        <v>29</v>
+      <c r="A40" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="5"/>
@@ -1114,7 +1129,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="5"/>
@@ -1122,7 +1137,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="5"/>
@@ -1130,7 +1145,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -1138,7 +1153,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -1152,7 +1167,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B46" s="4"/>
       <c r="C46" s="5"/>
@@ -1160,7 +1175,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="5"/>
@@ -1168,7 +1183,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B48" s="4"/>
       <c r="C48" s="5"/>
@@ -1176,7 +1191,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="5"/>
@@ -1184,7 +1199,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="5"/>
@@ -1197,8 +1212,8 @@
       <c r="D51" s="5"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="11" t="s">
-        <v>22</v>
+      <c r="A52" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -1206,7 +1221,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
@@ -1214,7 +1229,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>

</xml_diff>

<commit_message>
L E N  N  Y
</commit_message>
<xml_diff>
--- a/core/assets/levels/LevelTemplate.xlsx
+++ b/core/assets/levels/LevelTemplate.xlsx
@@ -372,7 +372,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -437,6 +437,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -464,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -482,10 +489,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,7 +774,7 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -869,10 +877,10 @@
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="14"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -951,8 +959,8 @@
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="4"/>
@@ -1037,6 +1045,7 @@
       <c r="D28" s="5"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -1074,7 +1083,7 @@
       <c r="D33" s="5"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="13" t="s">
         <v>55</v>
       </c>
       <c r="B34" s="4"/>

</xml_diff>

<commit_message>
still gotta test screm
</commit_message>
<xml_diff>
--- a/core/assets/levels/LevelTemplate.xlsx
+++ b/core/assets/levels/LevelTemplate.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
   <si>
     <t>Events</t>
   </si>
@@ -366,13 +366,16 @@
   </si>
   <si>
     <t>An average level is roughly 200 miles (40 rows total with normal padding).</t>
+  </si>
+  <si>
+    <t>Rear Enemy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -444,6 +447,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -468,8 +487,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -495,7 +516,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -774,7 +797,7 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -829,6 +852,9 @@
       <c r="D2" s="6" t="s">
         <v>50</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D3" s="6"/>
@@ -1261,5 +1287,6 @@
     <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
rest stop in progress pt 2
</commit_message>
<xml_diff>
--- a/core/assets/levels/LevelTemplate.xlsx
+++ b/core/assets/levels/LevelTemplate.xlsx
@@ -80,133 +80,167 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
+  <si>
+    <t>Middle Lane</t>
+  </si>
+  <si>
+    <t>Right Lane</t>
+  </si>
+  <si>
+    <t>Left Lane</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>SONGS:</t>
+  </si>
+  <si>
+    <t>Total number of blocks</t>
+  </si>
+  <si>
+    <t>Number of blocks to use:</t>
+  </si>
+  <si>
+    <t>Janky stuff we can change later:</t>
+  </si>
+  <si>
+    <t>To end the level, put "END" in the last row, in the events column</t>
+  </si>
+  <si>
+    <t>Upload up to 5 songs and include the file extension. Song files should be stored in assets/RadioSongs</t>
+  </si>
+  <si>
+    <t>Don't change number of lanes</t>
+  </si>
+  <si>
+    <t>Right now put 1 for total number of blocks and 1 for number of blocks to use</t>
+  </si>
+  <si>
+    <r>
+      <t>Speed:</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="13"/>
         <color theme="1"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>Events:</t>
-    </r>
-    <r>
-      <rPr>
+      <t xml:space="preserve"> Very slow, slow, normal, fast, very fast</t>
+    </r>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>If we make levels by shuffling random blocks:</t>
+  </si>
+  <si>
+    <t>Every block is (num lanes + 1) columns, beginning at column E.</t>
+  </si>
+  <si>
+    <t>To add a new block, copy the formatting of the block in the template beginning at the next column.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="13"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Rear Enemy, Sun, Ned wakes up, Nosh wakes up, SAT Question</t>
-    </r>
-  </si>
-  <si>
-    <t>File Name</t>
-  </si>
-  <si>
-    <t>END</t>
-  </si>
-  <si>
-    <t>Middle Lane</t>
-  </si>
-  <si>
-    <t>Right Lane</t>
-  </si>
-  <si>
-    <t>Left Lane</t>
-  </si>
-  <si>
-    <t>Speed</t>
-  </si>
-  <si>
-    <t>SONGS:</t>
-  </si>
-  <si>
-    <t>Total number of blocks</t>
-  </si>
-  <si>
-    <t>Number of blocks to use:</t>
-  </si>
-  <si>
-    <t>Janky stuff we can change later:</t>
-  </si>
-  <si>
-    <t>To end the level, put "END" in the last row, in the events column</t>
-  </si>
-  <si>
-    <t>Upload up to 5 songs and include the file extension. Song files should be stored in assets/RadioSongs</t>
-  </si>
-  <si>
-    <t>Don't change number of lanes</t>
-  </si>
-  <si>
-    <t>Right now put 1 for total number of blocks and 1 for number of blocks to use</t>
-  </si>
-  <si>
-    <r>
-      <t>Speed:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve"> Very slow, slow, normal, fast, very fast</t>
-    </r>
-  </si>
-  <si>
-    <t>Normal</t>
-  </si>
-  <si>
-    <t>If we make levels by shuffling random blocks:</t>
-  </si>
-  <si>
-    <t>Every block is (num lanes + 1) columns, beginning at column E.</t>
-  </si>
-  <si>
-    <t>To add a new block, copy the formatting of the block in the template beginning at the next column.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
+      <t>total number of blocks</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="13"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>total number of blocks</t>
-    </r>
-    <r>
-      <rPr>
+      <t xml:space="preserve"> field above should equal the total number of blocks you wrote in this doc.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="13"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> field above should equal the total number of blocks you wrote in this doc.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
+      <t>number of blocks to use</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="13"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>number of blocks to use</t>
+      <t xml:space="preserve"> field above should equal the number of blocks you want to select from the</t>
+    </r>
+  </si>
+  <si>
+    <t>total number of blocks. For example, you could define 25 total blocks but want to randomly select</t>
+  </si>
+  <si>
+    <t>10 blocks to build the actual level in-game. Then, the total number of blocks field would be 25,</t>
+  </si>
+  <si>
+    <t>and the number of blocks to use would be 10.</t>
+  </si>
+  <si>
+    <t>For example, for a 3-lane highway, each block is 4 columns wide.</t>
+  </si>
+  <si>
+    <t>TO ADD LATER: specify regions of the document and how many to select from each region</t>
+  </si>
+  <si>
+    <t>Padding between enemies:</t>
+  </si>
+  <si>
+    <r>
+      <t>Padding between enemies:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> Less, Normal, More</t>
+    </r>
+  </si>
+  <si>
+    <t>To end each block, still put "END" in the last row in the corresponding events column.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Enemies:</t>
     </r>
     <r>
       <rPr>
@@ -216,52 +250,21 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> field above should equal the number of blocks you want to select from the</t>
-    </r>
-  </si>
-  <si>
-    <t>total number of blocks. For example, you could define 25 total blocks but want to randomly select</t>
-  </si>
-  <si>
-    <t>10 blocks to build the actual level in-game. Then, the total number of blocks field would be 25,</t>
-  </si>
-  <si>
-    <t>and the number of blocks to use would be 10.</t>
-  </si>
-  <si>
-    <t>For example, for a 3-lane highway, each block is 4 columns wide.</t>
-  </si>
-  <si>
-    <t>TO ADD LATER: specify regions of the document and how many to select from each region</t>
-  </si>
-  <si>
-    <t>Padding between enemies:</t>
-  </si>
-  <si>
-    <r>
-      <t>Padding between enemies:</t>
-    </r>
-    <r>
-      <rPr>
+      <t xml:space="preserve"> Gnome, Grill, Flamingo</t>
+    </r>
+  </si>
+  <si>
+    <t>The Burbs</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
         <sz val="13"/>
         <color theme="1"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t xml:space="preserve"> Less, Normal, More</t>
-    </r>
-  </si>
-  <si>
-    <t>To end each block, still put "END" in the last row in the corresponding events column.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>Enemies:</t>
+      <t>Region:</t>
     </r>
     <r>
       <rPr>
@@ -271,78 +274,90 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Gnome, Grill, Flamingo</t>
-    </r>
-  </si>
-  <si>
-    <t>The Burbs</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
+      <t xml:space="preserve"> The Burbs, Highway, Midwest, Colorado </t>
+    </r>
+  </si>
+  <si>
+    <t>Randomly select blocks</t>
+  </si>
+  <si>
+    <t>Seed</t>
+  </si>
+  <si>
+    <r>
+      <t>Randomly select blocks</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="13"/>
         <color theme="1"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>Region:</t>
-    </r>
-    <r>
-      <rPr>
+      <t>: Yes or No</t>
+    </r>
+  </si>
+  <si>
+    <t>Seed is an integer used to randomly generate levels</t>
+  </si>
+  <si>
+    <t>If randomly select blocks is enabled, the specified number of blocks to use will be chosen randomly to build the level.</t>
+  </si>
+  <si>
+    <t>Otherwise, the blocks will be stitched together in order.</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="13"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> The Burbs, Highway, Midwest, Colorado </t>
-    </r>
-  </si>
-  <si>
-    <t>Randomly select blocks</t>
-  </si>
-  <si>
-    <t>Seed</t>
-  </si>
-  <si>
-    <r>
-      <t>Randomly select blocks</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>: Yes or No</t>
-    </r>
-  </si>
-  <si>
-    <t>Seed is an integer used to randomly generate levels</t>
-  </si>
-  <si>
-    <t>If randomly select blocks is enabled, the specified number of blocks to use will be chosen randomly to build the level.</t>
-  </si>
-  <si>
-    <t>Otherwise, the blocks will be stitched together in order.</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">For </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
+      <t>grills</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="13"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>grills</t>
+      <t>, specify when the grill flame starts ("Grill Starts") and where the grill spawns ("Grill End")</t>
+    </r>
+  </si>
+  <si>
+    <t>Grill Start</t>
+  </si>
+  <si>
+    <t>Grill End</t>
+  </si>
+  <si>
+    <t>Less padding: 1 cell = 3 miles / Normal padding: 1 cell = 5 miles / More padding: 1 cell = 8 miles</t>
+  </si>
+  <si>
+    <t>An average level is roughly 200 miles (40 rows total with normal padding).</t>
+  </si>
+  <si>
+    <t>Rear Enemy</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Events:</t>
     </r>
     <r>
       <rPr>
@@ -352,23 +367,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, specify when the grill flame starts ("Grill Starts") and where the grill spawns ("Grill End")</t>
-    </r>
-  </si>
-  <si>
-    <t>Grill Start</t>
-  </si>
-  <si>
-    <t>Grill End</t>
-  </si>
-  <si>
-    <t>Less padding: 1 cell = 3 miles / Normal padding: 1 cell = 5 miles / More padding: 1 cell = 8 miles</t>
-  </si>
-  <si>
-    <t>An average level is roughly 200 miles (40 rows total with normal padding).</t>
-  </si>
-  <si>
-    <t>Rear Enemy</t>
+      <t xml:space="preserve"> Rear Enemy, Sun Start/Sun End, Ned wakes up, Nosh wakes up, SAT Question</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -511,10 +511,10 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -796,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -818,42 +818,42 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="3">
         <v>3</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -861,16 +861,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>4</v>
@@ -890,7 +890,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="11">
         <v>0</v>
@@ -903,21 +903,21 @@
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="14"/>
+      <c r="A7" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="15"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" s="6"/>
       <c r="H8" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -938,7 +938,7 @@
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D12" s="6"/>
       <c r="H12" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -952,7 +952,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
@@ -986,7 +986,7 @@
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:7" ht="26" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="14" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="4"/>
@@ -1012,7 +1012,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
@@ -1020,7 +1020,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
@@ -1036,7 +1036,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
@@ -1044,18 +1044,18 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="5"/>
@@ -1086,7 +1086,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="5"/>
@@ -1094,7 +1094,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="5"/>
@@ -1102,7 +1102,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
@@ -1110,7 +1110,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="5"/>
@@ -1118,7 +1118,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="5"/>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="5"/>
@@ -1134,7 +1134,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="5"/>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="5"/>
@@ -1156,7 +1156,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="5"/>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="5"/>
@@ -1172,7 +1172,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="5"/>
@@ -1180,7 +1180,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -1188,7 +1188,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -1202,7 +1202,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B46" s="4"/>
       <c r="C46" s="5"/>
@@ -1210,7 +1210,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="5"/>
@@ -1218,7 +1218,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B48" s="4"/>
       <c r="C48" s="5"/>
@@ -1226,7 +1226,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="5"/>
@@ -1234,7 +1234,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="5"/>
@@ -1248,7 +1248,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -1256,7 +1256,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>

</xml_diff>